<commit_message>
finally got stock smart fig to work the way i wanted
</commit_message>
<xml_diff>
--- a/tables/TableS2_fmps.xlsx
+++ b/tables/TableS2_fmps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/us_fmps/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE99BC-0791-2544-939A-9A070A386149}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C386BD-3489-EF48-8389-2FCD55CE3560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12860" yWindow="2900" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19640" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,12 +347,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -367,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -382,6 +388,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +614,7 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -945,16 +956,16 @@
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="13" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="13" t="s">
@@ -965,19 +976,19 @@
       </c>
     </row>
     <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="13" t="s">
         <v>90</v>
       </c>
       <c r="F17" s="8">
@@ -985,19 +996,19 @@
       </c>
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="13" t="s">
         <v>68</v>
       </c>
       <c r="F18" s="8">
@@ -1005,19 +1016,19 @@
       </c>
     </row>
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F19" s="8">
@@ -1364,223 +1375,223 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36">
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="14">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="16">
         <v>1989</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37">
+    <row r="37" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="14">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="16">
         <v>2009</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38">
+    <row r="38" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="14">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="16">
         <v>1982</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39">
+    <row r="39" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="14">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="16">
         <v>1978</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40">
+    <row r="40" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="14">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="16">
         <v>1979</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41">
+    <row r="41" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="14">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="16">
         <v>1995</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42">
+    <row r="42" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="14">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="16">
         <v>2009</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43">
+    <row r="43" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="14">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="16">
         <v>2009</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44">
+    <row r="44" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="14">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="16">
         <v>2009</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45">
+    <row r="45" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="14">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="16">
         <v>2009</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46">
+    <row r="46" spans="1:6" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="14">
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="16">
         <v>2009</v>
       </c>
     </row>

</xml_diff>